<commit_message>
Initial commit, working version, transfered from lab pc
</commit_message>
<xml_diff>
--- a/MAC_List_test.xlsx
+++ b/MAC_List_test.xlsx
@@ -2045,8 +2045,8 @@
     <col width="13" bestFit="1" customWidth="1" style="14" min="12" max="13"/>
     <col width="82.28515625" bestFit="1" customWidth="1" style="97" min="14" max="14"/>
     <col width="255.5703125" bestFit="1" customWidth="1" style="14" min="15" max="15"/>
-    <col width="9.140625" customWidth="1" style="14" min="16" max="18"/>
-    <col width="9.140625" customWidth="1" style="14" min="19" max="16384"/>
+    <col width="9.140625" customWidth="1" style="14" min="16" max="25"/>
+    <col width="9.140625" customWidth="1" style="14" min="26" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="16">
@@ -9116,7 +9116,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD7"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9227,36 +9227,22 @@
         <f>IFERROR(_xlfn.IFNA(INDEX(Sensors_MANU!$E$2:$E$4692,MATCH($D2,Sensors_MANU!$B$2:$B$4692,0)),INDEX(Sensors_MANU!$E$2:$E$4692,MATCH($P2,Sensors_MANU!$A$2:$A$4692,0))),"")</f>
         <v/>
       </c>
-      <c r="B2" s="24">
-        <f>IFERROR(INDEX(Companies!$A$3:$A$101,MATCH(A2,Companies!$B$3:$B$101,0)),"")</f>
-        <v/>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Cargo</t>
-        </is>
-      </c>
+      <c r="B2" s="24" t="n"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>EC5EDE1E5DAC</t>
-        </is>
-      </c>
-      <c r="E2">
-        <f>LEFT(D2,2)&amp;":"&amp;MID(D2,3,2)&amp;":"&amp;MID(D2,5,2)&amp;":"&amp;MID(D2,7,2)&amp;":"&amp;MID(D2,9,2)&amp;":"&amp;RIGHT(D2,2)</f>
-        <v/>
+          <t>D2D9C24BBB2C</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>9BD0F696F03648E2</t>
-        </is>
-      </c>
-      <c r="I2" s="6">
-        <f>IFERROR(_xlfn.IFNA(INDEX(Sensors_MANU!$C$2:$C$4692,MATCH($D2,Sensors_MANU!$B$2:$B$4692,0)),INDEX(Sensors_MANU!$C$2:$C$4692,MATCH($P2,Sensors_MANU!$A$2:$A$4692,0))),"")</f>
-        <v/>
-      </c>
-      <c r="J2">
-        <f>IFERROR(_xlfn.IFNA(INDEX(Sensors_MANU!$D$2:$D$4692,MATCH($D2,Sensors_MANU!$B$2:$B$4692,0)),INDEX(Sensors_MANU!$D$2:$D$4692,MATCH($P2,Sensors_MANU!$A$2:$A$4692,0))),"")</f>
-        <v/>
+          <t>F1DCB0B324A7CA7B</t>
+        </is>
+      </c>
+      <c r="I2" s="6" t="n"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>F1DCB0B324A7CA7B</t>
+        </is>
       </c>
       <c r="K2" s="35" t="n"/>
       <c r="L2" s="35" t="n"/>
@@ -9276,22 +9262,7 @@
     </row>
     <row r="3">
       <c r="B3" s="24" t="n"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>FFD3024FF294</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>1CB77F4BF34E379E</t>
-        </is>
-      </c>
       <c r="I3" s="6" t="n"/>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>VIEZO1CB77F4BF34E379E</t>
-        </is>
-      </c>
       <c r="K3" s="35" t="n"/>
       <c r="L3" s="35" t="n"/>
       <c r="M3" s="35" t="n"/>
@@ -9299,41 +9270,11 @@
     </row>
     <row r="4">
       <c r="B4" s="24" t="n"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>F0842AA2C9A4</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>6771875AE0A36811</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>VIEZO6771875AE0A36811</t>
-        </is>
-      </c>
       <c r="M4" s="27" t="n"/>
       <c r="O4" s="6" t="n"/>
     </row>
     <row r="5">
       <c r="B5" s="24" t="n"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>F81E2490F9EC</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>08BE71E6F7DB7373</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>VIEZO08BE71E6F7DB7373</t>
-        </is>
-      </c>
       <c r="M5" s="27" t="n"/>
       <c r="O5" s="6" t="n"/>
     </row>

</xml_diff>